<commit_message>
:adhesive_bandage: Tentative patch for final upload
</commit_message>
<xml_diff>
--- a/outputs/Correlation_tests/rho_pvalue_matrix.xlsx
+++ b/outputs/Correlation_tests/rho_pvalue_matrix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20361"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20369"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mael\R_projects\ithomiini_current\outputs\Correlation_tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mael\R_projects\ithomiini_diversity\outputs\Correlation_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8BC06B-48E0-40FD-8523-6F0DA9DC7D46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D3BC41-ACBF-42C1-A7CB-EA76BD972AAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,16 +16,16 @@
     <sheet name="rho_pvalue_matrix" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Print_Area" localSheetId="0">rho_pvalue_matrix!$C$2:$M$12</definedName>
-    <definedName name="Rho_p_values_table" localSheetId="0">rho_pvalue_matrix!$C$2:$M$12</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">rho_pvalue_matrix!$C$2:$M$12</definedName>
+    <definedName name="Print_Area" localSheetId="0">rho_pvalue_matrix!$C$2:$M$13</definedName>
+    <definedName name="Rho_p_values_table" localSheetId="0">rho_pvalue_matrix!$C$2:$M$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">rho_pvalue_matrix!$C$2:$N$13</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="57">
   <si>
     <t>Sp. richness</t>
   </si>
@@ -39,12 +39,6 @@
     <t>Faith's PD</t>
   </si>
   <si>
-    <t>Sum of FP</t>
-  </si>
-  <si>
-    <t>MPD</t>
-  </si>
-  <si>
     <t>Mim. richness</t>
   </si>
   <si>
@@ -81,118 +75,127 @@
     <t>Rho coefficients</t>
   </si>
   <si>
-    <t>0.054</t>
-  </si>
-  <si>
-    <t>-0.314</t>
-  </si>
-  <si>
-    <t>0.073</t>
-  </si>
-  <si>
-    <t>0.099</t>
-  </si>
-  <si>
-    <t>0.05</t>
-  </si>
-  <si>
-    <t>0.078</t>
-  </si>
-  <si>
-    <t>0.101</t>
-  </si>
-  <si>
-    <t>-0.096</t>
-  </si>
-  <si>
-    <t>0.703</t>
-  </si>
-  <si>
-    <t>0.722</t>
-  </si>
-  <si>
-    <t>0.029*</t>
-  </si>
-  <si>
-    <t>0.607</t>
-  </si>
-  <si>
-    <t>0.498</t>
+    <t>ED</t>
+  </si>
+  <si>
+    <t>Mean ring size</t>
+  </si>
+  <si>
+    <t>Max ring size</t>
+  </si>
+  <si>
+    <t>0.941</t>
+  </si>
+  <si>
+    <t>0.948</t>
+  </si>
+  <si>
+    <t>0.934</t>
+  </si>
+  <si>
+    <t>0.891</t>
+  </si>
+  <si>
+    <t>0.995</t>
+  </si>
+  <si>
+    <t>0.943</t>
+  </si>
+  <si>
+    <t>0.949</t>
+  </si>
+  <si>
+    <t>0.931</t>
+  </si>
+  <si>
+    <t>0.887</t>
+  </si>
+  <si>
+    <t>0.94</t>
+  </si>
+  <si>
+    <t>0.945</t>
+  </si>
+  <si>
+    <t>0.924</t>
+  </si>
+  <si>
+    <t>0.936</t>
+  </si>
+  <si>
+    <t>0.897</t>
+  </si>
+  <si>
+    <t>0.957</t>
+  </si>
+  <si>
+    <t>0.784</t>
+  </si>
+  <si>
+    <t>0.733</t>
+  </si>
+  <si>
+    <t>0.811</t>
+  </si>
+  <si>
+    <t>0.734</t>
+  </si>
+  <si>
+    <t>0.981</t>
+  </si>
+  <si>
+    <t>0.473</t>
+  </si>
+  <si>
+    <t>0.475</t>
+  </si>
+  <si>
+    <t>0.46</t>
+  </si>
+  <si>
+    <t>0.42</t>
+  </si>
+  <si>
+    <t>0.433</t>
+  </si>
+  <si>
+    <t>0.417</t>
+  </si>
+  <si>
+    <t>0.379</t>
+  </si>
+  <si>
+    <t>0.606</t>
+  </si>
+  <si>
+    <t>0.604</t>
   </si>
   <si>
     <t>0.602</t>
   </si>
   <si>
-    <t>0.504</t>
-  </si>
-  <si>
-    <t>0.559</t>
-  </si>
-  <si>
-    <t>0.603</t>
-  </si>
-  <si>
-    <t>0.93</t>
-  </si>
-  <si>
-    <t>0.885</t>
-  </si>
-  <si>
-    <t>0.623</t>
-  </si>
-  <si>
-    <t>0.604</t>
-  </si>
-  <si>
-    <t>0.994</t>
-  </si>
-  <si>
-    <t>0.928</t>
-  </si>
-  <si>
-    <t>0.62</t>
-  </si>
-  <si>
-    <t>0.591</t>
-  </si>
-  <si>
-    <t>0.558</t>
-  </si>
-  <si>
-    <t>0.541</t>
-  </si>
-  <si>
-    <t>0.503</t>
-  </si>
-  <si>
-    <t>0.695</t>
-  </si>
-  <si>
-    <t>0.92</t>
-  </si>
-  <si>
-    <t>0.876</t>
-  </si>
-  <si>
-    <t>0.612</t>
-  </si>
-  <si>
-    <t>0.933</t>
-  </si>
-  <si>
-    <t>0.892</t>
-  </si>
-  <si>
-    <t>0.608</t>
-  </si>
-  <si>
-    <t>0.98</t>
-  </si>
-  <si>
-    <t>0.711</t>
-  </si>
-  <si>
-    <t>0.686</t>
+    <t>0.582</t>
+  </si>
+  <si>
+    <t>0.459</t>
+  </si>
+  <si>
+    <t>0.533</t>
+  </si>
+  <si>
+    <t>0.649</t>
+  </si>
+  <si>
+    <t>0.615</t>
+  </si>
+  <si>
+    <t>0.657</t>
+  </si>
+  <si>
+    <t>0.001**</t>
+  </si>
+  <si>
+    <t>0.002**</t>
   </si>
 </sst>
 </file>
@@ -715,27 +718,35 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -747,12 +758,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1112,10 +1117,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="C1:M12"/>
+  <dimension ref="C1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:M12"/>
+      <selection activeCell="C2" sqref="C2:N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1126,365 +1131,433 @@
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.42578125" customWidth="1"/>
     <col min="11" max="11" width="15.85546875" customWidth="1"/>
     <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="3:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="20" t="s">
+    <row r="1" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="3:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+    </row>
+    <row r="3" spans="3:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="6"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
+      <c r="I3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="3:13" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="10" t="s">
+    <row r="4" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="L3" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="10" t="s">
-        <v>8</v>
+      <c r="F4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C5" s="18"/>
+    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C5" s="20"/>
       <c r="D5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C6" s="20"/>
+      <c r="D6" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C7" s="20"/>
+      <c r="D7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="4" t="s">
+      <c r="F7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C8" s="20"/>
+      <c r="D8" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C9" s="20"/>
+      <c r="D9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C10" s="20"/>
+      <c r="D10" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C11" s="20"/>
+      <c r="D11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>15</v>
+      <c r="G11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C6" s="18"/>
-      <c r="D6" s="6" t="s">
+    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C12" s="20"/>
+      <c r="D12" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>15</v>
+      <c r="E12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C7" s="18"/>
-      <c r="D7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C8" s="18"/>
-      <c r="D8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C9" s="18"/>
-      <c r="D9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C10" s="18"/>
-      <c r="D10" s="6" t="s">
+    <row r="13" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="21"/>
+      <c r="D13" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10" s="2" t="s">
+      <c r="E13" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="G13" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="J10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C11" s="18"/>
-      <c r="D11" s="5" t="s">
+      <c r="J13" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="M13" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="N13" s="14" t="s">
         <v>7</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="19"/>
-      <c r="D12" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="I12" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="J12" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="K12" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="L12" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="M12" s="15" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C4:C12"/>
-    <mergeCell ref="E2:M2"/>
+    <mergeCell ref="C4:C13"/>
+    <mergeCell ref="E2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="95" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="87" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>